<commit_message>
add glasses and human signals
</commit_message>
<xml_diff>
--- a/code/energy in the signals.xlsx
+++ b/code/energy in the signals.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="360" yWindow="510" windowWidth="10215" windowHeight="4305"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
   <si>
     <t>windmill</t>
   </si>
@@ -44,24 +47,33 @@
   </si>
   <si>
     <t>Let-It-Go Violin</t>
+  </si>
+  <si>
+    <t>crystalglass</t>
+  </si>
+  <si>
+    <t>heartmonitor-ekg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <sz val="15.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
@@ -71,7 +83,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -86,71 +98,348 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kontortema">
+  <a:themeElements>
+    <a:clrScheme name="Kontor">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Kontor">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Kontor">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="18.57"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -159,7 +448,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -176,31 +465,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="1">
-        <v>41414.0</v>
+        <v>41414</v>
       </c>
       <c r="B11" s="1">
-        <v>41414.0</v>
+        <v>41414</v>
       </c>
       <c r="C11" s="1">
         <v>710.0009</v>
       </c>
       <c r="D11" s="1">
-        <v>41414.0</v>
+        <v>41414</v>
       </c>
       <c r="E11" s="1">
-        <v>17926.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>17926</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -209,7 +498,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -226,32 +515,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="3">
-        <v>30731.0</v>
+        <v>30731</v>
       </c>
       <c r="B15" s="3">
-        <v>30731.0</v>
+        <v>30731</v>
       </c>
       <c r="C15" s="3">
-        <v>686.3515</v>
+        <v>686.35149999999999</v>
       </c>
       <c r="D15" s="3">
-        <v>30731.0</v>
+        <v>30731</v>
       </c>
       <c r="E15" s="3">
-        <v>13389.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>13389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -268,29 +557,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="3">
-        <v>134470.0</v>
+        <v>134470</v>
       </c>
       <c r="B20" s="3">
-        <v>134470.0</v>
+        <v>134470</v>
       </c>
       <c r="C20" s="3">
-        <v>1292.0</v>
+        <v>1292</v>
       </c>
       <c r="D20" s="3">
-        <v>134470.0</v>
+        <v>134470</v>
       </c>
       <c r="E20" s="3">
-        <v>73893.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>73893</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -307,24 +596,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="3">
-        <v>298310.0</v>
+        <v>298310</v>
       </c>
       <c r="B24" s="3">
-        <v>298310.0</v>
+        <v>298310</v>
       </c>
       <c r="C24" s="3">
         <v>1698.9</v>
       </c>
       <c r="D24" s="3">
-        <v>298310.0</v>
+        <v>298310</v>
       </c>
       <c r="E24" s="3">
-        <v>128470.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>128470</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -333,7 +622,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -350,29 +639,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="1">
-        <v>162720.0</v>
+        <v>162720</v>
       </c>
       <c r="B28" s="1">
-        <v>162720.0</v>
+        <v>162720</v>
       </c>
       <c r="C28" s="1">
         <v>1726.8</v>
       </c>
       <c r="D28" s="1">
-        <v>162720.0</v>
+        <v>162720</v>
       </c>
       <c r="E28" s="1">
-        <v>68616.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>68616</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
@@ -389,24 +678,102 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="3">
-        <v>22377.0</v>
+        <v>22377</v>
       </c>
       <c r="B32" s="3">
-        <v>22377.0</v>
+        <v>22377</v>
       </c>
       <c r="C32" s="2">
-        <v>896.4634</v>
+        <v>896.46339999999998</v>
       </c>
       <c r="D32" s="3">
-        <v>22377.0</v>
+        <v>22377</v>
       </c>
       <c r="E32" s="3">
-        <v>10933.0</v>
+        <v>10933</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A36" s="6">
+        <v>115.2349</v>
+      </c>
+      <c r="B36" s="6">
+        <v>115.2349</v>
+      </c>
+      <c r="C36" s="6">
+        <v>154.83199999999999</v>
+      </c>
+      <c r="D36" s="6">
+        <v>115.2349</v>
+      </c>
+      <c r="E36" s="6">
+        <v>2.6453000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A40" s="7">
+        <v>20489</v>
+      </c>
+      <c r="B40" s="7">
+        <v>20489</v>
+      </c>
+      <c r="C40" s="5">
+        <v>625.85699999999997</v>
+      </c>
+      <c r="D40" s="7">
+        <v>20489</v>
+      </c>
+      <c r="E40" s="7">
+        <v>7294.9</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>